<commit_message>
update shopping list confirm
</commit_message>
<xml_diff>
--- a/public/downloads/stocklist_example_data.xlsx
+++ b/public/downloads/stocklist_example_data.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
+  <workbookPr filterPrivacy="1"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9660"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -77,75 +80,24 @@
   </si>
   <si>
     <t>21</t>
-  </si>
-  <si>
-    <t>Aspirne</t>
-  </si>
-  <si>
-    <t>Tablets</t>
-  </si>
-  <si>
-    <t>Mg</t>
-  </si>
-  <si>
-    <t>aspirne</t>
-  </si>
-  <si>
-    <t>73827</t>
-  </si>
-  <si>
-    <t>2017-03-23</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Bleomycin sulfate</t>
-  </si>
-  <si>
-    <t>vial</t>
-  </si>
-  <si>
-    <t>IU</t>
-  </si>
-  <si>
-    <t>BLEO 15K</t>
-  </si>
-  <si>
-    <t>Amneal Pharma Australia Pty Ltd</t>
-  </si>
-  <si>
-    <t>2736</t>
-  </si>
-  <si>
-    <t>2014-07-22</t>
-  </si>
-  <si>
-    <t>ARTG</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>Bleomycin test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -518,11 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="66"/>
+    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -534,7 +488,7 @@
     <col min="14" max="14" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,134 +576,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3">
-        <v>2000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3">
-        <v>20</v>
-      </c>
-      <c r="L3">
-        <v>20</v>
-      </c>
-      <c r="M3">
-        <v>20</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>15000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>32</v>
-      </c>
-      <c r="M4">
-        <v>23</v>
-      </c>
-      <c r="N4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>207</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>15000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>32</v>
-      </c>
-      <c r="M5">
-        <v>23</v>
-      </c>
-      <c r="N5" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>